<commit_message>
modulo upload agentes por excel se permite subir sucursales.
</commit_message>
<xml_diff>
--- a/rest-api/tmpExcel/Ejemplo-Lista-Agentes.xlsx
+++ b/rest-api/tmpExcel/Ejemplo-Lista-Agentes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp3\htdocs\duocMVC\rest-api\tmpExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp4\htdocs\SocioClaveMVC\rest-api\tmpExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6891C8E4-0122-47E7-864B-6563AA0913CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B847ABBF-E2C0-422E-88EB-CE4E1F35DCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>RUT</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>CORREO</t>
+  </si>
+  <si>
+    <t>DIRECCION</t>
+  </si>
+  <si>
+    <t>CELULAR</t>
+  </si>
+  <si>
+    <t>SUCURSALES (cod sucursal separado por ,)</t>
   </si>
 </sst>
 </file>
@@ -49,15 +58,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="2"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="2"/>
+      <sz val="9"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,7 +81,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -94,10 +103,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,18 +387,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -399,8 +409,17 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>

</xml_diff>